<commit_message>
ajout des diagrammes de comparaison des IA d'Assistance
</commit_message>
<xml_diff>
--- a/documents/8-Iteration6/Comparaison_IA_Deduction/comparaison_IA_Deduction.xlsx
+++ b/documents/8-Iteration6/Comparaison_IA_Deduction/comparaison_IA_Deduction.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enzom\OneDrive\Documents\BUT-Informatique\BUT3\Projet Tutoré\SAE_Kronologic_Dietrich_Dziezuk_Mougin\documents\9-Comparaison_IA_Deduction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enzom\OneDrive\Documents\BUT-Informatique\BUT3\Projet Tutoré\SAE_Kronologic_Dietrich_Dziezuk_Mougin\documents\8-Iteration6\Comparaison_IA_Deduction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCD5D29-6A91-4FC7-88AC-0AD9AD092185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A04DC4-5181-46D7-AC06-694D796E79A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D48D6D2E-15DA-470C-9B34-0D45AB2DB35E}"/>
   </bookViews>
@@ -1595,8 +1595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADABEBDF-14B1-42A6-BBA8-E19A1E152D23}">
   <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C14" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2127,7 +2127,7 @@
       <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <f>AVERAGE(B2:B11)</f>
         <v>90.202119999999994</v>
       </c>
@@ -2174,7 +2174,7 @@
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <f>MAX(B2:B11)</f>
         <v>103.1644</v>
       </c>
@@ -2221,7 +2221,7 @@
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <f>MIN(B2:B11)</f>
         <v>80.017899999999997</v>
       </c>

</xml_diff>